<commit_message>
Changed ESC to GESC (grave + Esc) to make Tilde entry easier
</commit_message>
<xml_diff>
--- a/Notes and scripts/Ctrl layout help sheet.xlsx
+++ b/Notes and scripts/Ctrl layout help sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liam2/Documents/QMK/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liam2/Documents/GitHub/qmk_firmware/Notes and scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0E17DB-8BF8-5B44-95CE-635AF2F9454A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CBD6E9-48E0-F844-A073-8797415FA5B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="1160" windowWidth="27640" windowHeight="16940" activeTab="3" xr2:uid="{A6F6E149-121B-F84A-9B42-431FA814CB94}"/>
+    <workbookView xWindow="7940" yWindow="1000" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{A6F6E149-121B-F84A-9B42-431FA814CB94}"/>
   </bookViews>
   <sheets>
     <sheet name="Zone map" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="161">
   <si>
     <t>led:104</t>
   </si>
@@ -401,12 +401,6 @@
     <t>space: 80</t>
   </si>
   <si>
-    <t>f2: 3</t>
-  </si>
-  <si>
-    <t>f1: 2</t>
-  </si>
-  <si>
     <t>f3: 4</t>
   </si>
   <si>
@@ -431,12 +425,6 @@
     <t>f10: 11</t>
   </si>
   <si>
-    <t>f11: 12</t>
-  </si>
-  <si>
-    <t>f12 : 13</t>
-  </si>
-  <si>
     <t>led: 104</t>
   </si>
   <si>
@@ -461,9 +449,6 @@
     <t>led: 111</t>
   </si>
   <si>
-    <t>led: 112</t>
-  </si>
-  <si>
     <t>led: 113</t>
   </si>
   <si>
@@ -491,12 +476,6 @@
     <t>pause: 16</t>
   </si>
   <si>
-    <t>-: 28</t>
-  </si>
-  <si>
-    <t>"=": 29</t>
-  </si>
-  <si>
     <t>backspace: 30</t>
   </si>
   <si>
@@ -509,31 +488,40 @@
     <t>1: 18</t>
   </si>
   <si>
-    <t>2: 19</t>
-  </si>
-  <si>
-    <t>3: 20</t>
-  </si>
-  <si>
-    <t>4: 21</t>
-  </si>
-  <si>
-    <t>5: 22</t>
-  </si>
-  <si>
-    <t>6: 23</t>
-  </si>
-  <si>
-    <t>7: 24</t>
-  </si>
-  <si>
-    <t>8: 25</t>
-  </si>
-  <si>
-    <t>9: 26</t>
-  </si>
-  <si>
-    <t>0: 27</t>
+    <t>f1: 1</t>
+  </si>
+  <si>
+    <t>f1: 3</t>
+  </si>
+  <si>
+    <t>f11: 11</t>
+  </si>
+  <si>
+    <t>f11 : 13</t>
+  </si>
+  <si>
+    <t>-: 18</t>
+  </si>
+  <si>
+    <t>"=": 19</t>
+  </si>
+  <si>
+    <t>home: 31</t>
+  </si>
+  <si>
+    <t>i: 41</t>
+  </si>
+  <si>
+    <t>a: 51</t>
+  </si>
+  <si>
+    <t>" : 61</t>
+  </si>
+  <si>
+    <t>, : 71</t>
+  </si>
+  <si>
+    <t>fn: 81</t>
   </si>
 </sst>
 </file>
@@ -712,7 +700,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -756,6 +744,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -775,6 +766,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1544,10 +1538,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1557,43 +1551,43 @@
   <sheetData>
     <row r="1" spans="1:20" s="14" customFormat="1">
       <c r="A1" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="M1" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="N1" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>139</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="P1" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="S1" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="T1" s="13" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="25" customHeight="1">
@@ -1642,54 +1636,54 @@
         <v>13</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F3" s="9" t="s">
+      <c r="H3" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="K3" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="L3" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="M3" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="L3" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>129</v>
-      </c>
       <c r="N3" s="9" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="S3" s="9" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="25" customHeight="1">
       <c r="B4" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="11">
         <v>1</v>
@@ -1704,16 +1698,16 @@
         <v>1</v>
       </c>
       <c r="H4" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K4" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L4" s="11">
         <v>1</v>
@@ -1728,72 +1722,72 @@
         <v>1</v>
       </c>
       <c r="Q4" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R4" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S4" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="14" customFormat="1">
       <c r="A5" s="13" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="25">
+        <v>5.486111111111111E-2</v>
+      </c>
+      <c r="E5" s="25">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="F5" s="25">
+        <v>0.17430555555555555</v>
+      </c>
+      <c r="G5" s="25">
+        <v>0.21597222222222223</v>
+      </c>
+      <c r="H5" s="25">
+        <v>0.2590277777777778</v>
+      </c>
+      <c r="I5" s="25">
+        <v>0.30138888888888887</v>
+      </c>
+      <c r="J5" s="25">
+        <v>0.34375</v>
+      </c>
+      <c r="K5" s="25">
+        <v>0.38611111111111113</v>
+      </c>
+      <c r="L5" s="25">
+        <v>1.1805555555555555E-2</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="O5" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q5" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="R5" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="N5" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="O5" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q5" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="R5" s="13" t="s">
-        <v>35</v>
-      </c>
       <c r="S5" s="13" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="T5" s="13" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="25" customHeight="1">
@@ -1840,16 +1834,16 @@
         <v>1</v>
       </c>
       <c r="O6" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q6" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R6" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S6" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T6" s="11">
         <v>1</v>
@@ -1857,7 +1851,7 @@
     </row>
     <row r="7" spans="1:20" s="14" customFormat="1">
       <c r="A7" s="13" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>39</v>
@@ -1884,7 +1878,7 @@
         <v>46</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>47</v>
+        <v>156</v>
       </c>
       <c r="K7" s="13" t="s">
         <v>48</v>
@@ -1919,7 +1913,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="11">
         <v>1</v>
@@ -1961,13 +1955,13 @@
         <v>1</v>
       </c>
       <c r="Q8" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R8" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S8" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T8" s="11">
         <v>1</v>
@@ -1981,7 +1975,7 @@
         <v>58</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>59</v>
+        <v>157</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>60</v>
@@ -2011,12 +2005,12 @@
         <v>68</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="N9" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="N9" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="O9" s="19"/>
+      <c r="O9" s="20"/>
       <c r="T9" s="13" t="s">
         <v>71</v>
       </c>
@@ -2026,7 +2020,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="11">
         <v>1</v>
@@ -2061,19 +2055,19 @@
       <c r="M10" s="11">
         <v>1</v>
       </c>
-      <c r="N10" s="20">
-        <v>2</v>
-      </c>
-      <c r="O10" s="22"/>
+      <c r="N10" s="21">
+        <v>1</v>
+      </c>
+      <c r="O10" s="23"/>
       <c r="T10" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:20" s="14" customFormat="1">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="19"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="13" t="s">
         <v>73</v>
       </c>
@@ -2096,7 +2090,7 @@
         <v>79</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>80</v>
+        <v>159</v>
       </c>
       <c r="L11" s="13" t="s">
         <v>81</v>
@@ -2104,19 +2098,19 @@
       <c r="M11" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="N11" s="17" t="s">
+      <c r="N11" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="O11" s="19"/>
+      <c r="O11" s="20"/>
       <c r="R11" s="13" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="25" customHeight="1">
-      <c r="B12" s="20">
-        <v>2</v>
-      </c>
-      <c r="C12" s="22"/>
+      <c r="B12" s="21">
+        <v>1</v>
+      </c>
+      <c r="C12" s="23"/>
       <c r="D12" s="11">
         <v>1</v>
       </c>
@@ -2147,12 +2141,12 @@
       <c r="M12" s="11">
         <v>1</v>
       </c>
-      <c r="N12" s="20">
-        <v>2</v>
-      </c>
-      <c r="O12" s="22"/>
+      <c r="N12" s="21">
+        <v>1</v>
+      </c>
+      <c r="O12" s="23"/>
       <c r="R12" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:20" s="14" customFormat="1">
@@ -2165,20 +2159,20 @@
       <c r="D13" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="20"/>
       <c r="L13" s="13" t="s">
         <v>89</v>
       </c>
       <c r="M13" s="13" t="s">
-        <v>90</v>
+        <v>160</v>
       </c>
       <c r="N13" s="13" t="s">
         <v>91</v>
@@ -2198,43 +2192,43 @@
     </row>
     <row r="14" spans="1:20" ht="25" customHeight="1">
       <c r="B14" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="11">
-        <v>2</v>
-      </c>
-      <c r="E14" s="20">
-        <v>1</v>
-      </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="22"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="21">
+        <v>1</v>
+      </c>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="23"/>
       <c r="L14" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M14" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N14" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O14" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q14" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R14" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S14" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:20" s="14" customFormat="1">
@@ -2263,7 +2257,7 @@
         <v>103</v>
       </c>
       <c r="M15" s="13" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N15" s="13" t="s">
         <v>105</v>
@@ -2318,6 +2312,9 @@
       <c r="T16" s="11">
         <v>1</v>
       </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2351,7 +2348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A09C0BFF-9F47-7B4D-9825-8CAA87F69F2E}">
   <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
+    <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
@@ -2368,14 +2365,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="12" t="s">
@@ -2415,7 +2412,7 @@
       </c>
       <c r="B3">
         <f>Layout!B4</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2425,11 +2422,11 @@
       </c>
       <c r="F3">
         <f>COUNTIF($B3,F$2)*POWER(2,$D3)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:K3" si="0">COUNTIF($B3,G$2)*POWER(2,$D3)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <f t="shared" si="0"/>
@@ -2610,7 +2607,7 @@
       </c>
       <c r="B8">
         <f ca="1">OFFSET(Layout!$D$4,0,4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2620,11 +2617,11 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="1"/>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="1"/>
@@ -2649,7 +2646,7 @@
       </c>
       <c r="B9">
         <f ca="1">OFFSET(Layout!$D$4,0,5)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -2659,11 +2656,11 @@
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="1"/>
@@ -2688,7 +2685,7 @@
       </c>
       <c r="B10">
         <f ca="1">OFFSET(Layout!$D$4,0,6)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -2698,11 +2695,11 @@
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="1"/>
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="1"/>
@@ -2727,7 +2724,7 @@
       </c>
       <c r="B11">
         <f ca="1">OFFSET(Layout!$D$4,0,7)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2737,11 +2734,11 @@
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>256</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="1"/>
-        <v>256</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="1"/>
@@ -2922,7 +2919,7 @@
       </c>
       <c r="B16">
         <f>Layout!Q4</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2932,11 +2929,11 @@
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8192</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
-        <v>8192</v>
+        <v>0</v>
       </c>
       <c r="H16">
         <f t="shared" si="1"/>
@@ -2961,7 +2958,7 @@
       </c>
       <c r="B17">
         <f>Layout!R4</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2971,11 +2968,11 @@
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>16384</v>
       </c>
       <c r="G17">
         <f t="shared" si="1"/>
-        <v>16384</v>
+        <v>0</v>
       </c>
       <c r="H17">
         <f t="shared" si="1"/>
@@ -3000,7 +2997,7 @@
       </c>
       <c r="B18">
         <f>Layout!S4</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -3010,11 +3007,11 @@
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>32768</v>
       </c>
       <c r="G18">
         <f t="shared" si="1"/>
-        <v>32768</v>
+        <v>0</v>
       </c>
       <c r="H18">
         <f t="shared" si="1"/>
@@ -3546,7 +3543,7 @@
       </c>
       <c r="B32">
         <f ca="1">OFFSET(Layout!$B$6,0,13)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3556,11 +3553,11 @@
       </c>
       <c r="F32">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>536870912</v>
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="1"/>
-        <v>536870912</v>
+        <v>0</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="1"/>
@@ -3585,7 +3582,7 @@
       </c>
       <c r="B33">
         <f>Layout!Q6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -3595,11 +3592,11 @@
       </c>
       <c r="F33">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1073741824</v>
       </c>
       <c r="G33">
         <f t="shared" si="1"/>
-        <v>1073741824</v>
+        <v>0</v>
       </c>
       <c r="H33">
         <f t="shared" si="1"/>
@@ -3624,7 +3621,7 @@
       </c>
       <c r="B34">
         <f>Layout!R6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -3634,11 +3631,11 @@
       </c>
       <c r="F34">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2147483648</v>
       </c>
       <c r="G34">
         <f t="shared" si="1"/>
-        <v>2147483648</v>
+        <v>0</v>
       </c>
       <c r="H34">
         <f t="shared" si="1"/>
@@ -3663,7 +3660,7 @@
       </c>
       <c r="B35">
         <f>Layout!S6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -3673,11 +3670,11 @@
       </c>
       <c r="F35">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35">
         <f t="shared" si="1"/>
@@ -3702,7 +3699,7 @@
       </c>
       <c r="B36">
         <f>Layout!B8</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -3712,11 +3709,11 @@
       </c>
       <c r="F36">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G36">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H36">
         <f t="shared" si="1"/>
@@ -4248,7 +4245,7 @@
       </c>
       <c r="B50">
         <f>Layout!Q8</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C50">
         <v>2</v>
@@ -4258,11 +4255,11 @@
       </c>
       <c r="F50">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>32768</v>
       </c>
       <c r="G50">
         <f t="shared" si="2"/>
-        <v>32768</v>
+        <v>0</v>
       </c>
       <c r="H50">
         <f t="shared" si="2"/>
@@ -4287,7 +4284,7 @@
       </c>
       <c r="B51">
         <f>Layout!R8</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C51">
         <v>2</v>
@@ -4297,11 +4294,11 @@
       </c>
       <c r="F51">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>65536</v>
       </c>
       <c r="G51">
         <f t="shared" si="2"/>
-        <v>65536</v>
+        <v>0</v>
       </c>
       <c r="H51">
         <f t="shared" si="2"/>
@@ -4326,7 +4323,7 @@
       </c>
       <c r="B52">
         <f>Layout!S8</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C52">
         <v>2</v>
@@ -4336,11 +4333,11 @@
       </c>
       <c r="F52">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>131072</v>
       </c>
       <c r="G52">
         <f t="shared" si="2"/>
-        <v>131072</v>
+        <v>0</v>
       </c>
       <c r="H52">
         <f t="shared" si="2"/>
@@ -4365,7 +4362,7 @@
       </c>
       <c r="B53">
         <f>Layout!B10</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C53">
         <v>2</v>
@@ -4375,11 +4372,11 @@
       </c>
       <c r="F53">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>262144</v>
       </c>
       <c r="G53">
         <f t="shared" si="2"/>
-        <v>262144</v>
+        <v>0</v>
       </c>
       <c r="H53">
         <f t="shared" si="2"/>
@@ -4833,7 +4830,7 @@
       </c>
       <c r="B65">
         <f ca="1">OFFSET(Layout!$B$10,0,12)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C65">
         <v>2</v>
@@ -4843,11 +4840,11 @@
       </c>
       <c r="F65">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1073741824</v>
       </c>
       <c r="G65">
         <f t="shared" ca="1" si="3"/>
-        <v>1073741824</v>
+        <v>0</v>
       </c>
       <c r="H65">
         <f t="shared" ca="1" si="3"/>
@@ -4872,7 +4869,7 @@
       </c>
       <c r="B66">
         <f>Layout!B12</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C66">
         <v>2</v>
@@ -4882,11 +4879,11 @@
       </c>
       <c r="F66">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2147483648</v>
       </c>
       <c r="G66">
         <f t="shared" si="3"/>
-        <v>2147483648</v>
+        <v>0</v>
       </c>
       <c r="H66">
         <f t="shared" si="3"/>
@@ -5301,7 +5298,7 @@
       </c>
       <c r="B77">
         <f ca="1">OFFSET(Layout!$B$12,0,12)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C77">
         <v>3</v>
@@ -5311,11 +5308,11 @@
       </c>
       <c r="F77">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1024</v>
       </c>
       <c r="G77">
         <f t="shared" ca="1" si="4"/>
-        <v>1024</v>
+        <v>0</v>
       </c>
       <c r="H77">
         <f t="shared" ca="1" si="4"/>
@@ -5340,7 +5337,7 @@
       </c>
       <c r="B78">
         <f>Layout!R12</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C78">
         <v>3</v>
@@ -5350,11 +5347,11 @@
       </c>
       <c r="F78">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2048</v>
       </c>
       <c r="G78">
         <f t="shared" si="4"/>
-        <v>2048</v>
+        <v>0</v>
       </c>
       <c r="H78">
         <f t="shared" si="4"/>
@@ -5379,7 +5376,7 @@
       </c>
       <c r="B79">
         <f>Layout!B14</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C79">
         <v>3</v>
@@ -5389,11 +5386,11 @@
       </c>
       <c r="F79">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4096</v>
       </c>
       <c r="G79">
         <f t="shared" si="4"/>
-        <v>4096</v>
+        <v>0</v>
       </c>
       <c r="H79">
         <f t="shared" si="4"/>
@@ -5418,7 +5415,7 @@
       </c>
       <c r="B80">
         <f ca="1">OFFSET(Layout!$B$14,0,1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C80">
         <v>3</v>
@@ -5428,11 +5425,11 @@
       </c>
       <c r="F80">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>8192</v>
       </c>
       <c r="G80">
         <f t="shared" ca="1" si="4"/>
-        <v>8192</v>
+        <v>0</v>
       </c>
       <c r="H80">
         <f t="shared" ca="1" si="4"/>
@@ -5457,7 +5454,7 @@
       </c>
       <c r="B81">
         <f ca="1">OFFSET(Layout!$B$14,0,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C81">
         <v>3</v>
@@ -5467,11 +5464,11 @@
       </c>
       <c r="F81">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>16384</v>
       </c>
       <c r="G81">
         <f t="shared" ca="1" si="4"/>
-        <v>16384</v>
+        <v>0</v>
       </c>
       <c r="H81">
         <f t="shared" ca="1" si="4"/>
@@ -5535,7 +5532,7 @@
       </c>
       <c r="B83">
         <f>Layout!L14</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C83">
         <v>3</v>
@@ -5545,11 +5542,11 @@
       </c>
       <c r="F83">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>65536</v>
       </c>
       <c r="G83">
         <f t="shared" si="4"/>
-        <v>65536</v>
+        <v>0</v>
       </c>
       <c r="H83">
         <f t="shared" si="4"/>
@@ -5574,7 +5571,7 @@
       </c>
       <c r="B84">
         <f ca="1">OFFSET(Layout!$L$14,0,1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C84">
         <v>3</v>
@@ -5584,11 +5581,11 @@
       </c>
       <c r="F84">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>131072</v>
       </c>
       <c r="G84">
         <f t="shared" ca="1" si="4"/>
-        <v>131072</v>
+        <v>0</v>
       </c>
       <c r="H84">
         <f t="shared" ca="1" si="4"/>
@@ -5613,7 +5610,7 @@
       </c>
       <c r="B85">
         <f ca="1">OFFSET(Layout!$L$14,0,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C85">
         <v>3</v>
@@ -5623,11 +5620,11 @@
       </c>
       <c r="F85">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>262144</v>
       </c>
       <c r="G85">
         <f t="shared" ca="1" si="4"/>
-        <v>262144</v>
+        <v>0</v>
       </c>
       <c r="H85">
         <f t="shared" ca="1" si="4"/>
@@ -5652,7 +5649,7 @@
       </c>
       <c r="B86">
         <f ca="1">OFFSET(Layout!$L$14,0,3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C86">
         <v>3</v>
@@ -5662,11 +5659,11 @@
       </c>
       <c r="F86">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>524288</v>
       </c>
       <c r="G86">
         <f t="shared" ca="1" si="4"/>
-        <v>524288</v>
+        <v>0</v>
       </c>
       <c r="H86">
         <f t="shared" ca="1" si="4"/>
@@ -5691,7 +5688,7 @@
       </c>
       <c r="B87">
         <f ca="1">OFFSET(Layout!$L$14,0,5)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C87">
         <v>3</v>
@@ -5701,11 +5698,11 @@
       </c>
       <c r="F87">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1048576</v>
       </c>
       <c r="G87">
         <f t="shared" ca="1" si="4"/>
-        <v>1048576</v>
+        <v>0</v>
       </c>
       <c r="H87">
         <f t="shared" ca="1" si="4"/>
@@ -5730,7 +5727,7 @@
       </c>
       <c r="B88">
         <f ca="1">OFFSET(Layout!$L$14,0,6)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C88">
         <v>3</v>
@@ -5740,11 +5737,11 @@
       </c>
       <c r="F88">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>2097152</v>
       </c>
       <c r="G88">
         <f t="shared" ca="1" si="4"/>
-        <v>2097152</v>
+        <v>0</v>
       </c>
       <c r="H88">
         <f t="shared" ca="1" si="4"/>
@@ -5769,7 +5766,7 @@
       </c>
       <c r="B89">
         <f ca="1">OFFSET(Layout!$L$14,0,7)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C89">
         <v>3</v>
@@ -5779,11 +5776,11 @@
       </c>
       <c r="F89">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>4194304</v>
       </c>
       <c r="G89">
         <f t="shared" ca="1" si="4"/>
-        <v>4194304</v>
+        <v>0</v>
       </c>
       <c r="H89">
         <f t="shared" ca="1" si="4"/>
@@ -7074,8 +7071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F1FBC6-0864-0145-9FA6-4A5CBA82821E}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7110,15 +7107,15 @@
       </c>
       <c r="B2">
         <f ca="1">SUM(Calcs!F$3:F$34)</f>
-        <v>536813086</v>
+        <v>4294967295</v>
       </c>
       <c r="C2">
         <f ca="1">SUM(Calcs!F$35:F$66)</f>
-        <v>1073250300</v>
+        <v>4294967295</v>
       </c>
       <c r="D2">
         <f ca="1">SUM(Calcs!F$67:F$98)</f>
-        <v>4286612479</v>
+        <v>4294967295</v>
       </c>
       <c r="E2">
         <f ca="1">SUM(Calcs!F$99:F$121)</f>
@@ -7126,7 +7123,7 @@
       </c>
       <c r="G2" t="str">
         <f ca="1">_xlfn.CONCAT(".id0 = ", B2, ", .id1 = ", C2, ", .id2 = ", D2, ", .id3 = ", E2)</f>
-        <v>.id0 = 536813086, .id1 = 1073250300, .id2 = 4286612479, .id3 = 8388607</v>
+        <v>.id0 = 4294967295, .id1 = 4294967295, .id2 = 4294967295, .id3 = 8388607</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -7135,15 +7132,15 @@
       </c>
       <c r="B3">
         <f ca="1">SUM(Calcs!G$3:G$34)</f>
-        <v>3758154209</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <f ca="1">SUM(Calcs!G$35:G$66)</f>
-        <v>3221716995</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <f ca="1">SUM(Calcs!G$67:G$98)</f>
-        <v>8354816</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <f ca="1">SUM(Calcs!G$99:G$121)</f>
@@ -7151,7 +7148,7 @@
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G7" ca="1" si="0">_xlfn.CONCAT(".id0 = ", B3, ", .id1 = ", C3, ", .id2 = ", D3, ", .id3 = ", E3)</f>
-        <v>.id0 = 3758154209, .id1 = 3221716995, .id2 = 8354816, .id3 = 0</v>
+        <v>.id0 = 0, .id1 = 0, .id2 = 0, .id3 = 0</v>
       </c>
     </row>
     <row r="4" spans="1:7">

</xml_diff>